<commit_message>
logic before provisioning api
</commit_message>
<xml_diff>
--- a/api_layer/sample_sharepack.xlsx
+++ b/api_layer/sample_sharepack.xlsx
@@ -20,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -30,10 +30,13 @@
     </font>
     <font>
       <b val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
       <color rgb="00FFFFFF"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="6">
     <fill>
       <patternFill/>
     </fill>
@@ -44,6 +47,24 @@
       <patternFill patternType="solid">
         <fgColor rgb="004472C4"/>
         <bgColor rgb="004472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0070AD47"/>
+        <bgColor rgb="0070AD47"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFC000"/>
+        <bgColor rgb="00FFC000"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E7E6E6"/>
+        <bgColor rgb="00E7E6E6"/>
       </patternFill>
     </fill>
   </fills>
@@ -59,9 +80,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -427,7 +457,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -435,8 +465,8 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="50" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="60" customWidth="1" min="2" max="2"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -508,6 +538,90 @@
       <c r="B6" t="inlineStr">
         <is>
           <t>Test share pack for workflow validation</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>delta_share_region</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>AM</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>configurator</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>data-platform-team@jll.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>approver</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>analytics-leadership@jll.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>executive_team</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>data-governance-team@jll.com</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>approver_status</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>approved</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>workspace_url</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>https://adb-1234567890123456.12.azuredatabricks.net</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>contact_email</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>test.user@jll.com</t>
         </is>
       </c>
     </row>
@@ -522,7 +636,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -530,41 +644,53 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="8" customWidth="1" min="2" max="2"/>
-    <col width="25" customWidth="1" min="3" max="3"/>
-    <col width="30" customWidth="1" min="4" max="4"/>
-    <col width="30" customWidth="1" min="5" max="5"/>
-    <col width="40" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="1" max="1"/>
+    <col width="18" customWidth="1" min="2" max="2"/>
+    <col width="18" customWidth="1" min="3" max="3"/>
+    <col width="18" customWidth="1" min="4" max="4"/>
+    <col width="18" customWidth="1" min="5" max="5"/>
+    <col width="18" customWidth="1" min="6" max="6"/>
+    <col width="18" customWidth="1" min="7" max="7"/>
+    <col width="18" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
+      <c r="A1" s="2" t="inlineStr">
         <is>
           <t>name</t>
         </is>
       </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="B1" s="2" t="inlineStr">
         <is>
           <t>type</t>
         </is>
       </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>email</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>metastore_id</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>allowed_ips</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>recipient</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>recipient_databricks_org</t>
+        </is>
+      </c>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>recipient_ips</t>
+        </is>
+      </c>
+      <c r="F1" s="2" t="inlineStr">
+        <is>
+          <t>token_expiry</t>
+        </is>
+      </c>
+      <c r="G1" s="2" t="inlineStr">
+        <is>
+          <t>token_rotation</t>
+        </is>
+      </c>
+      <c r="H1" s="2" t="inlineStr">
         <is>
           <t>comment</t>
         </is>
@@ -583,16 +709,23 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>test@example.com</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr"/>
+          <t>test-recipient@example.com</t>
+        </is>
+      </c>
       <c r="E2" t="inlineStr">
         <is>
           <t>192.168.1.0/24,10.0.0.50</t>
         </is>
       </c>
-      <c r="F2" t="inlineStr">
+      <c r="F2" t="n">
+        <v>30</v>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
         <is>
           <t>Test D2O recipient for validation</t>
         </is>
@@ -609,14 +742,17 @@
           <t>D2D</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr"/>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>d2d-recipient@example.com</t>
+        </is>
+      </c>
       <c r="D3" t="inlineStr">
         <is>
           <t>aws:us-west-2:abc-123-def-456</t>
         </is>
       </c>
-      <c r="E3" t="inlineStr"/>
-      <c r="F3" t="inlineStr">
+      <c r="H3" t="inlineStr">
         <is>
           <t>Test D2D recipient for validation</t>
         </is>
@@ -633,7 +769,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -641,31 +777,55 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="25" customWidth="1" min="2" max="2"/>
-    <col width="50" customWidth="1" min="3" max="3"/>
-    <col width="60" customWidth="1" min="4" max="4"/>
+    <col width="22" customWidth="1" min="1" max="1"/>
+    <col width="22" customWidth="1" min="2" max="2"/>
+    <col width="22" customWidth="1" min="3" max="3"/>
+    <col width="22" customWidth="1" min="4" max="4"/>
+    <col width="22" customWidth="1" min="5" max="5"/>
+    <col width="22" customWidth="1" min="6" max="6"/>
+    <col width="22" customWidth="1" min="7" max="7"/>
+    <col width="22" customWidth="1" min="8" max="8"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>share_name</t>
+        </is>
+      </c>
+      <c r="B1" s="3" t="inlineStr">
+        <is>
+          <t>asset</t>
+        </is>
+      </c>
+      <c r="C1" s="3" t="inlineStr">
+        <is>
+          <t>recipient</t>
+        </is>
+      </c>
+      <c r="D1" s="3" t="inlineStr">
+        <is>
+          <t>ext_catalog_name</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>ext_schema_name</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="inlineStr">
+        <is>
+          <t>prefix_assetname</t>
+        </is>
+      </c>
+      <c r="G1" s="3" t="inlineStr">
+        <is>
+          <t>share_tags</t>
+        </is>
+      </c>
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>comment</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>recipients</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>data_objects</t>
         </is>
       </c>
     </row>
@@ -677,39 +837,212 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Q1 test data share</t>
+          <t>catalog.schema.sales_data</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>test-recipient-d2o,test-recipient-d2d</t>
+          <t>test-recipient-d2o</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>catalog.schema.test_table_1,catalog.schema.test_table_2</t>
+          <t>target_catalog</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>target_schema</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>prod_</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>production,q1_analytics</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>Q1 test data share - individual table assets</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
+          <t>test_share_q1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>catalog.schema.customer_data</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>test-recipient-d2d</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>target_catalog</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>target_schema</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>prod_</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>production,q1_analytics</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>test_share_q1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>catalog.schema.product_view</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>target_catalog</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>target_schema</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>prod_</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>production,q1_analytics</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
           <t>test_audit_share</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Test audit logs</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>catalog.audit_schema.activity_log</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
         <is>
           <t>test-recipient-d2o</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>catalog.audit_schema.activity_log</t>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>audit_target_catalog</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>audit_target_schema</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>rt_</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>production,compliance</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>Audit schema share - all tables in schema with individual pipelines</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>test_audit_share</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>catalog.audit_schema.error_log</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>audit_target_catalog</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>audit_target_schema</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>rt_</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>production,compliance</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>test_audit_share</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>catalog.audit_schema.access_log</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>audit_target_catalog</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>audit_target_schema</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>rt_</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>production,compliance</t>
         </is>
       </c>
     </row>
@@ -724,7 +1057,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F1"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -733,42 +1066,384 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
     <col width="20" customWidth="1" min="1" max="1"/>
-    <col width="15" customWidth="1" min="2" max="2"/>
+    <col width="20" customWidth="1" min="2" max="2"/>
     <col width="20" customWidth="1" min="3" max="3"/>
-    <col width="40" customWidth="1" min="4" max="4"/>
-    <col width="40" customWidth="1" min="5" max="5"/>
-    <col width="40" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="20" customWidth="1" min="5" max="5"/>
+    <col width="20" customWidth="1" min="6" max="6"/>
+    <col width="20" customWidth="1" min="7" max="7"/>
+    <col width="20" customWidth="1" min="8" max="8"/>
+    <col width="20" customWidth="1" min="9" max="9"/>
+    <col width="20" customWidth="1" min="10" max="10"/>
+    <col width="20" customWidth="1" min="11" max="11"/>
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>type</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>schedule</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>source</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>destination</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>comment</t>
+      <c r="A1" s="4" t="inlineStr">
+        <is>
+          <t>share_name</t>
+        </is>
+      </c>
+      <c r="B1" s="4" t="inlineStr">
+        <is>
+          <t>name_prefix</t>
+        </is>
+      </c>
+      <c r="C1" s="4" t="inlineStr">
+        <is>
+          <t>asset_name</t>
+        </is>
+      </c>
+      <c r="D1" s="4" t="inlineStr">
+        <is>
+          <t>schedule_type</t>
+        </is>
+      </c>
+      <c r="E1" s="4" t="inlineStr">
+        <is>
+          <t>cron</t>
+        </is>
+      </c>
+      <c r="F1" s="4" t="inlineStr">
+        <is>
+          <t>timezone</t>
+        </is>
+      </c>
+      <c r="G1" s="4" t="inlineStr">
+        <is>
+          <t>scd_type</t>
+        </is>
+      </c>
+      <c r="H1" s="4" t="inlineStr">
+        <is>
+          <t>key_columns</t>
+        </is>
+      </c>
+      <c r="I1" s="4" t="inlineStr">
+        <is>
+          <t>serverless</t>
+        </is>
+      </c>
+      <c r="J1" s="4" t="inlineStr">
+        <is>
+          <t>notification</t>
+        </is>
+      </c>
+      <c r="K1" s="4" t="inlineStr">
+        <is>
+          <t>tags</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>test_share_q1</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>q1_sync_pipeline_sales</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>catalog.schema.sales_data</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>CRON</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>0 0 2 * * ?</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>America/New_York</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>sale_id,timestamp</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J2" t="inlineStr">
+        <is>
+          <t>analytics-team@jll.com</t>
+        </is>
+      </c>
+      <c r="K2" t="inlineStr">
+        <is>
+          <t>environment:production,dataset:sales</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>test_share_q1</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>q1_sync_pipeline_customer</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>catalog.schema.customer_data</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>CRON</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>0 0 */6 * * ?</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>UTC</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>customer_id,updated_at</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>false</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>analytics-team@jll.com</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>environment:production,dataset:customer</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>test_share_q1</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>q1_sync_pipeline_product</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>catalog.schema.product_view</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>CRON</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>0 0 * * * ?</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>UTC</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>analytics-team@jll.com</t>
+        </is>
+      </c>
+      <c r="K4" t="inlineStr">
+        <is>
+          <t>environment:production,dataset:product</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>test_audit_share</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>audit_sync_pipeline_1</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>catalog.audit_schema.activity_log</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>CONTINUOUS</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J5" t="inlineStr">
+        <is>
+          <t>audit-team@jll.com</t>
+        </is>
+      </c>
+      <c r="K5" t="inlineStr">
+        <is>
+          <t>environment:production,table:activity_log</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>test_audit_share</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>audit_sync_pipeline_2</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>catalog.audit_schema.error_log</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>CRON</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>0 */15 * * * ?</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>UTC</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J6" t="inlineStr">
+        <is>
+          <t>audit-team@jll.com</t>
+        </is>
+      </c>
+      <c r="K6" t="inlineStr">
+        <is>
+          <t>environment:production,table:error_log</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>test_audit_share</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>audit_sync_pipeline_3</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>catalog.audit_schema.access_log</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>CRON</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>0 0 * * * ?</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>UTC</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>true</t>
+        </is>
+      </c>
+      <c r="J7" t="inlineStr">
+        <is>
+          <t>audit-team@jll.com</t>
+        </is>
+      </c>
+      <c r="K7" t="inlineStr">
+        <is>
+          <t>environment:production,table:access_log</t>
         </is>
       </c>
     </row>

</xml_diff>